<commit_message>
Changed log values to base 2
</commit_message>
<xml_diff>
--- a/Ex6/Ex6-RatioAnalysis.xlsx
+++ b/Ex6/Ex6-RatioAnalysis.xlsx
@@ -539,7 +539,7 @@
   <dimension ref="B2:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,11 +627,11 @@
         <v>9.0600000000000007E-5</v>
       </c>
       <c r="E4" s="2">
-        <f>B4</f>
+        <f t="shared" ref="E4:E11" si="0">B4</f>
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <f>LOG10(E4)</f>
+        <f>LOG(E4,2)</f>
         <v>0</v>
       </c>
       <c r="G4" s="2">
@@ -647,23 +647,23 @@
         <v>1</v>
       </c>
       <c r="J4" s="2">
-        <f>C4/E4</f>
+        <f t="shared" ref="J4:J11" si="1">C4/E4</f>
         <v>0</v>
       </c>
       <c r="K4" s="2" t="e">
-        <f>C4/F4</f>
+        <f t="shared" ref="K4:K11" si="2">C4/F4</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L4" s="2" t="e">
-        <f>C4/G4</f>
+        <f t="shared" ref="L4:L11" si="3">C4/G4</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M4" s="2">
-        <f>C4/H4</f>
+        <f t="shared" ref="M4:M11" si="4">C4/H4</f>
         <v>0</v>
       </c>
       <c r="N4" s="2">
-        <f>C4/I4</f>
+        <f t="shared" ref="N4:N11" si="5">C4/I4</f>
         <v>0</v>
       </c>
     </row>
@@ -678,43 +678,43 @@
         <v>9.1899999999999903E-5</v>
       </c>
       <c r="E5" s="2">
-        <f>B5</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F11" si="0">LOG10(E5)</f>
-        <v>1</v>
+        <f t="shared" ref="F5:F11" si="6">LOG(E5,2)</f>
+        <v>3.3219280948873626</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ref="G5:G11" si="1">E5*F5</f>
-        <v>10</v>
+        <f t="shared" ref="G5:G11" si="7">E5*F5</f>
+        <v>33.219280948873624</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ref="H5:H11" si="2">POWER(E5,2)</f>
+        <f t="shared" ref="H5:H11" si="8">POWER(E5,2)</f>
         <v>100</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" ref="I5:I11" si="3">POWER(E5, 3)</f>
+        <f t="shared" ref="I5:I11" si="9">POWER(E5, 3)</f>
         <v>1000</v>
       </c>
       <c r="J5" s="2">
-        <f>C5/E5</f>
+        <f t="shared" si="1"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="K5" s="2">
-        <f>C5/F5</f>
-        <v>23</v>
+        <f t="shared" si="2"/>
+        <v>6.9236899002715671</v>
       </c>
       <c r="L5" s="2">
-        <f>C5/G5</f>
-        <v>2.2999999999999998</v>
+        <f t="shared" si="3"/>
+        <v>0.69236899002715668</v>
       </c>
       <c r="M5" s="2">
-        <f>C5/H5</f>
+        <f t="shared" si="4"/>
         <v>0.23</v>
       </c>
       <c r="N5" s="2">
-        <f>C5/I5</f>
+        <f t="shared" si="5"/>
         <v>2.3E-2</v>
       </c>
     </row>
@@ -729,43 +729,43 @@
         <v>3.611E-4</v>
       </c>
       <c r="E6" s="2">
-        <f>B6</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="0"/>
-        <v>1.6989700043360187</v>
+        <f t="shared" si="6"/>
+        <v>5.6438561897747244</v>
       </c>
       <c r="G6" s="2">
+        <f t="shared" si="7"/>
+        <v>282.1928094887362</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="8"/>
+        <v>2500</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="9"/>
+        <v>125000</v>
+      </c>
+      <c r="J6" s="2">
         <f t="shared" si="1"/>
-        <v>84.948500216800937</v>
-      </c>
-      <c r="H6" s="2">
+        <v>4.42</v>
+      </c>
+      <c r="K6" s="2">
         <f t="shared" si="2"/>
-        <v>2500</v>
-      </c>
-      <c r="I6" s="2">
+        <v>39.157624249958303</v>
+      </c>
+      <c r="L6" s="2">
         <f t="shared" si="3"/>
-        <v>125000</v>
-      </c>
-      <c r="J6" s="2">
-        <f>C6/E6</f>
-        <v>4.42</v>
-      </c>
-      <c r="K6" s="2">
-        <f>C6/F6</f>
-        <v>130.07881212497915</v>
-      </c>
-      <c r="L6" s="2">
-        <f>C6/G6</f>
-        <v>2.6015762424995832</v>
+        <v>0.78315248499916601</v>
       </c>
       <c r="M6" s="2">
-        <f>C6/H6</f>
+        <f t="shared" si="4"/>
         <v>8.8400000000000006E-2</v>
       </c>
       <c r="N6" s="2">
-        <f>C6/I6</f>
+        <f t="shared" si="5"/>
         <v>1.768E-3</v>
       </c>
     </row>
@@ -780,43 +780,43 @@
         <v>7.3450000000000002E-4</v>
       </c>
       <c r="E7" s="2">
-        <f>B7</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="6"/>
+        <v>6.6438561897747253</v>
       </c>
       <c r="G7" s="2">
+        <f t="shared" si="7"/>
+        <v>664.38561897747252</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="9"/>
+        <v>1000000</v>
+      </c>
+      <c r="J7" s="2">
         <f t="shared" si="1"/>
-        <v>200</v>
-      </c>
-      <c r="H7" s="2">
+        <v>5.35</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="2"/>
-        <v>10000</v>
-      </c>
-      <c r="I7" s="2">
+        <v>80.525523840114957</v>
+      </c>
+      <c r="L7" s="2">
         <f t="shared" si="3"/>
-        <v>1000000</v>
-      </c>
-      <c r="J7" s="2">
-        <f>C7/E7</f>
-        <v>5.35</v>
-      </c>
-      <c r="K7" s="2">
-        <f>C7/F7</f>
-        <v>267.5</v>
-      </c>
-      <c r="L7" s="2">
-        <f>C7/G7</f>
-        <v>2.6749999999999998</v>
+        <v>0.80525523840114965</v>
       </c>
       <c r="M7" s="2">
-        <f>C7/H7</f>
+        <f t="shared" si="4"/>
         <v>5.3499999999999999E-2</v>
       </c>
       <c r="N7" s="2">
-        <f>C7/I7</f>
+        <f t="shared" si="5"/>
         <v>5.3499999999999999E-4</v>
       </c>
     </row>
@@ -831,43 +831,43 @@
         <v>4.07209999999999E-3</v>
       </c>
       <c r="E8" s="2">
-        <f>B8</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="0"/>
-        <v>2.6989700043360187</v>
+        <f t="shared" si="6"/>
+        <v>8.965784284662087</v>
       </c>
       <c r="G8" s="2">
+        <f t="shared" si="7"/>
+        <v>4482.8921423310439</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="9"/>
+        <v>125000000</v>
+      </c>
+      <c r="J8" s="2">
         <f t="shared" si="1"/>
-        <v>1349.4850021680095</v>
-      </c>
-      <c r="H8" s="2">
+        <v>7.71</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="2"/>
-        <v>250000</v>
-      </c>
-      <c r="I8" s="2">
+        <v>429.9679623783511</v>
+      </c>
+      <c r="L8" s="2">
         <f t="shared" si="3"/>
-        <v>125000000</v>
-      </c>
-      <c r="J8" s="2">
-        <f>C8/E8</f>
-        <v>7.71</v>
-      </c>
-      <c r="K8" s="2">
-        <f>C8/F8</f>
-        <v>1428.3226541261172</v>
-      </c>
-      <c r="L8" s="2">
-        <f>C8/G8</f>
-        <v>2.8566453082522338</v>
+        <v>0.85993592475670222</v>
       </c>
       <c r="M8" s="2">
-        <f>C8/H8</f>
+        <f t="shared" si="4"/>
         <v>1.542E-2</v>
       </c>
       <c r="N8" s="2">
-        <f>C8/I8</f>
+        <f t="shared" si="5"/>
         <v>3.0840000000000003E-5</v>
       </c>
     </row>
@@ -882,43 +882,43 @@
         <v>1.8904499999999901E-2</v>
       </c>
       <c r="E9" s="2">
-        <f>B9</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>9.965784284662087</v>
       </c>
       <c r="G9" s="2">
+        <f t="shared" si="7"/>
+        <v>9965.7842846620879</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="8"/>
+        <v>1000000</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="9"/>
+        <v>1000000000</v>
+      </c>
+      <c r="J9" s="2">
         <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-      <c r="H9" s="2">
+        <v>8.7210000000000001</v>
+      </c>
+      <c r="K9" s="2">
         <f t="shared" si="2"/>
-        <v>1000000</v>
-      </c>
-      <c r="I9" s="2">
+        <v>875.09419739519331</v>
+      </c>
+      <c r="L9" s="2">
         <f t="shared" si="3"/>
-        <v>1000000000</v>
-      </c>
-      <c r="J9" s="2">
-        <f>C9/E9</f>
-        <v>8.7210000000000001</v>
-      </c>
-      <c r="K9" s="2">
-        <f>C9/F9</f>
-        <v>2907</v>
-      </c>
-      <c r="L9" s="2">
-        <f>C9/G9</f>
-        <v>2.907</v>
+        <v>0.87509419739519323</v>
       </c>
       <c r="M9" s="2">
-        <f>C9/H9</f>
+        <f t="shared" si="4"/>
         <v>8.7209999999999996E-3</v>
       </c>
       <c r="N9" s="2">
-        <f>C9/I9</f>
+        <f t="shared" si="5"/>
         <v>8.721E-6</v>
       </c>
     </row>
@@ -933,43 +933,43 @@
         <v>4.7044299999999997E-2</v>
       </c>
       <c r="E10" s="2">
-        <f>B10</f>
+        <f t="shared" si="0"/>
         <v>5000</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="0"/>
-        <v>3.6989700043360187</v>
+        <f t="shared" si="6"/>
+        <v>12.287712379549451</v>
       </c>
       <c r="G10" s="2">
+        <f t="shared" si="7"/>
+        <v>61438.561897747255</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="8"/>
+        <v>25000000</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="9"/>
+        <v>125000000000</v>
+      </c>
+      <c r="J10" s="2">
         <f t="shared" si="1"/>
-        <v>18494.850021680093</v>
-      </c>
-      <c r="H10" s="2">
+        <v>11.0402</v>
+      </c>
+      <c r="K10" s="2">
         <f t="shared" si="2"/>
-        <v>25000000</v>
-      </c>
-      <c r="I10" s="2">
+        <v>4492.374031465085</v>
+      </c>
+      <c r="L10" s="2">
         <f t="shared" si="3"/>
-        <v>125000000000</v>
-      </c>
-      <c r="J10" s="2">
-        <f>C10/E10</f>
-        <v>11.0402</v>
-      </c>
-      <c r="K10" s="2">
-        <f>C10/F10</f>
-        <v>14923.343507866271</v>
-      </c>
-      <c r="L10" s="2">
-        <f>C10/G10</f>
-        <v>2.9846687015732543</v>
+        <v>0.89847480629301701</v>
       </c>
       <c r="M10" s="2">
-        <f>C10/H10</f>
+        <f t="shared" si="4"/>
         <v>2.2080400000000001E-3</v>
       </c>
       <c r="N10" s="2">
-        <f>C10/I10</f>
+        <f t="shared" si="5"/>
         <v>4.4160799999999999E-7</v>
       </c>
     </row>
@@ -984,43 +984,43 @@
         <v>0.104303799999999</v>
       </c>
       <c r="E11" s="2">
-        <f>B11</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>13.287712379549451</v>
       </c>
       <c r="G11" s="2">
+        <f t="shared" si="7"/>
+        <v>132877.1237954945</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="8"/>
+        <v>100000000</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="9"/>
+        <v>1000000000000</v>
+      </c>
+      <c r="J11" s="2">
         <f t="shared" si="1"/>
-        <v>40000</v>
-      </c>
-      <c r="H11" s="2">
+        <v>12.047700000000001</v>
+      </c>
+      <c r="K11" s="2">
         <f t="shared" si="2"/>
-        <v>100000000</v>
-      </c>
-      <c r="I11" s="2">
+        <v>9066.7976969023657</v>
+      </c>
+      <c r="L11" s="2">
         <f t="shared" si="3"/>
-        <v>1000000000000</v>
-      </c>
-      <c r="J11" s="2">
-        <f>C11/E11</f>
-        <v>12.047700000000001</v>
-      </c>
-      <c r="K11" s="2">
-        <f>C11/F11</f>
-        <v>30119.25</v>
-      </c>
-      <c r="L11" s="2">
-        <f>C11/G11</f>
-        <v>3.0119250000000002</v>
+        <v>0.90667976969023656</v>
       </c>
       <c r="M11" s="2">
-        <f>C11/H11</f>
+        <f t="shared" si="4"/>
         <v>1.20477E-3</v>
       </c>
       <c r="N11" s="2">
-        <f>C11/I11</f>
+        <f t="shared" si="5"/>
         <v>1.20477E-7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added ratio analysis for binary search
</commit_message>
<xml_diff>
--- a/Ex6/Ex6-RatioAnalysis.xlsx
+++ b/Ex6/Ex6-RatioAnalysis.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\DSALabEx5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PyCharmProjects\DSALab\Ex6\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A172D1-9D89-419C-9357-1F56D322E47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Merge Sort" sheetId="4" r:id="rId1"/>
+    <sheet name="Binary Search" sheetId="6" r:id="rId1"/>
+    <sheet name="Merge Sort" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Degree(n)</t>
   </si>
@@ -145,11 +147,14 @@
   <si>
     <t>Execution time</t>
   </si>
+  <si>
+    <t>Ratio Analysis of Binary Search</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -535,30 +540,501 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6EDF7F-5FB0-4BFD-8637-C8A341252F56}">
+  <dimension ref="B2:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="2:13" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <f>B4</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <f>LOG(D4,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <f>D4*E4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <f>POWER(D4,2)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <f>POWER(D4, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <f>C4/D4</f>
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <f>C4/E4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K4" s="2" t="e">
+        <f>C4/F4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L4" s="2">
+        <f>C4/G4</f>
+        <v>2</v>
+      </c>
+      <c r="M4" s="2">
+        <f>C4/H4</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <f>B5</f>
+        <v>10</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E11" si="0">LOG(D5,2)</f>
+        <v>3.3219280948873626</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F11" si="1">D5*E5</f>
+        <v>33.219280948873624</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G11" si="2">POWER(D5,2)</f>
+        <v>100</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" ref="H5:H11" si="3">POWER(D5, 3)</f>
+        <v>1000</v>
+      </c>
+      <c r="I5" s="2">
+        <f>C5/D5</f>
+        <v>0.8</v>
+      </c>
+      <c r="J5" s="2">
+        <f>C5/E5</f>
+        <v>2.4082399653118491</v>
+      </c>
+      <c r="K5" s="2">
+        <f>C5/F5</f>
+        <v>0.24082399653118494</v>
+      </c>
+      <c r="L5" s="2">
+        <f>C5/G5</f>
+        <v>0.08</v>
+      </c>
+      <c r="M5" s="2">
+        <f>C5/H5</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2">
+        <f>B6</f>
+        <v>50</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>5.6438561897747244</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="1"/>
+        <v>282.1928094887362</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="2"/>
+        <v>2500</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="3"/>
+        <v>125000</v>
+      </c>
+      <c r="I6" s="2">
+        <f>C6/D6</f>
+        <v>0.22</v>
+      </c>
+      <c r="J6" s="2">
+        <f>C6/E6</f>
+        <v>1.9490220214911371</v>
+      </c>
+      <c r="K6" s="2">
+        <f>C6/F6</f>
+        <v>3.8980440429822745E-2</v>
+      </c>
+      <c r="L6" s="2">
+        <f>C6/G6</f>
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="M6" s="2">
+        <f>C6/H6</f>
+        <v>8.7999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>100</v>
+      </c>
+      <c r="C7" s="2">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2">
+        <f>B7</f>
+        <v>100</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>6.6438561897747253</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>664.38561897747252</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>10000</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="3"/>
+        <v>1000000</v>
+      </c>
+      <c r="I7" s="2">
+        <f>C7/D7</f>
+        <v>0.17</v>
+      </c>
+      <c r="J7" s="2">
+        <f>C7/E7</f>
+        <v>2.5587549631438398</v>
+      </c>
+      <c r="K7" s="2">
+        <f>C7/F7</f>
+        <v>2.5587549631438399E-2</v>
+      </c>
+      <c r="L7" s="2">
+        <f>C7/G7</f>
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="M7" s="2">
+        <f>C7/H7</f>
+        <v>1.7E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>500</v>
+      </c>
+      <c r="C8" s="2">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2">
+        <f>B8</f>
+        <v>500</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>8.965784284662087</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>4482.8921423310439</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="2"/>
+        <v>250000</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="3"/>
+        <v>125000000</v>
+      </c>
+      <c r="I8" s="2">
+        <f>C8/D8</f>
+        <v>0.04</v>
+      </c>
+      <c r="J8" s="2">
+        <f>C8/E8</f>
+        <v>2.2307027879551291</v>
+      </c>
+      <c r="K8" s="2">
+        <f>C8/F8</f>
+        <v>4.4614055759102577E-3</v>
+      </c>
+      <c r="L8" s="2">
+        <f>C8/G8</f>
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="M8" s="2">
+        <f>C8/H8</f>
+        <v>1.6E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2">
+        <f>B9</f>
+        <v>1000</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>9.965784284662087</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>9965.7842846620879</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>1000000</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="3"/>
+        <v>1000000000</v>
+      </c>
+      <c r="I9" s="2">
+        <f>C9/D9</f>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="J9" s="2">
+        <f>C9/E9</f>
+        <v>2.909956624751818</v>
+      </c>
+      <c r="K9" s="2">
+        <f>C9/F9</f>
+        <v>2.909956624751818E-3</v>
+      </c>
+      <c r="L9" s="2">
+        <f>C9/G9</f>
+        <v>2.9E-5</v>
+      </c>
+      <c r="M9" s="2">
+        <f>C9/H9</f>
+        <v>2.9000000000000002E-8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>5000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2">
+        <f>B10</f>
+        <v>5000</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>12.287712379549451</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>61438.561897747255</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>25000000</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="3"/>
+        <v>125000000000</v>
+      </c>
+      <c r="I10" s="2">
+        <f>C10/D10</f>
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="J10" s="2">
+        <f>C10/E10</f>
+        <v>2.360081283173991</v>
+      </c>
+      <c r="K10" s="2">
+        <f>C10/F10</f>
+        <v>4.7201625663479817E-4</v>
+      </c>
+      <c r="L10" s="2">
+        <f>C10/G10</f>
+        <v>1.1599999999999999E-6</v>
+      </c>
+      <c r="M10" s="2">
+        <f>C10/H10</f>
+        <v>2.32E-10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2">
+        <f>B11</f>
+        <v>10000</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>13.287712379549451</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
+        <v>132877.1237954945</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>100000000</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="3"/>
+        <v>1000000000000</v>
+      </c>
+      <c r="I11" s="2">
+        <f>C11/D11</f>
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="J11" s="2">
+        <f>C11/E11</f>
+        <v>2.6340124620598351</v>
+      </c>
+      <c r="K11" s="2">
+        <f>C11/F11</f>
+        <v>2.6340124620598352E-4</v>
+      </c>
+      <c r="L11" s="2">
+        <f>C11/G11</f>
+        <v>3.4999999999999998E-7</v>
+      </c>
+      <c r="M11" s="2">
+        <f>C11/H11</f>
+        <v>3.5000000000000002E-11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" customWidth="1"/>
+    <col min="3" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
@@ -575,7 +1051,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="2:14" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -667,7 +1143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>10</v>
       </c>
@@ -718,7 +1194,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>50</v>
       </c>
@@ -769,7 +1245,7 @@
         <v>1.768E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>100</v>
       </c>
@@ -820,7 +1296,7 @@
         <v>5.3499999999999999E-4</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>500</v>
       </c>
@@ -871,7 +1347,7 @@
         <v>3.0840000000000003E-5</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>1000</v>
       </c>
@@ -922,7 +1398,7 @@
         <v>8.721E-6</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>5000</v>
       </c>
@@ -973,7 +1449,7 @@
         <v>4.4160799999999999E-7</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>10000</v>
       </c>
@@ -1024,7 +1500,7 @@
         <v>1.20477E-7</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1035,7 +1511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1043,7 +1519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1051,11 +1527,11 @@
         <v>9.4900000000008798E-5</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1066,7 +1542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
         <v>15</v>
       </c>
@@ -1074,7 +1550,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
added ratio analysis for quicksort
</commit_message>
<xml_diff>
--- a/Ex6/Ex6-RatioAnalysis.xlsx
+++ b/Ex6/Ex6-RatioAnalysis.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PyCharmProjects\DSALab\Ex6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A172D1-9D89-419C-9357-1F56D322E47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1E1103-B0A8-4A97-B88C-0A092326758D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Binary Search" sheetId="6" r:id="rId1"/>
-    <sheet name="Merge Sort" sheetId="4" r:id="rId2"/>
+    <sheet name="Quick Sort" sheetId="7" r:id="rId1"/>
+    <sheet name="Binary Search" sheetId="6" r:id="rId2"/>
+    <sheet name="Merge Sort" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
   <si>
     <t>Degree(n)</t>
   </si>
@@ -150,6 +151,9 @@
   <si>
     <t>Ratio Analysis of Binary Search</t>
   </si>
+  <si>
+    <t>Ratio Analysis of Quick Sort</t>
+  </si>
 </sst>
 </file>
 
@@ -214,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,6 +231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +545,481 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4B8617-E7DD-49C2-A5D1-CBD21F772CFB}">
+  <dimension ref="B2:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="2:13" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D11" si="0">B4</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <f>LOG(D4,2)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <f>D4*E4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <f>POWER(D4,2)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <f>POWER(D4, 3)</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I11" si="1">C4/D4</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <f t="shared" ref="J4:J11" si="2">C4/E4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K4" s="2" t="e">
+        <f t="shared" ref="K4:K11" si="3">C4/F4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:L11" si="4">C4/G4</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" ref="M4:M11" si="5">C4/H4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>56</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E11" si="6">LOG(D5,2)</f>
+        <v>3.3219280948873626</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F11" si="7">D5*E5</f>
+        <v>33.219280948873624</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G11" si="8">POWER(D5,2)</f>
+        <v>100</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" ref="H5:H11" si="9">POWER(D5, 3)</f>
+        <v>1000</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>5.6</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="2"/>
+        <v>16.857679757182947</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="3"/>
+        <v>1.6857679757182946</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="4"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="5"/>
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2">
+        <v>341</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="6"/>
+        <v>5.6438561897747244</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="7"/>
+        <v>282.1928094887362</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="8"/>
+        <v>2500</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="9"/>
+        <v>125000</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="1"/>
+        <v>6.82</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="2"/>
+        <v>60.419682666225249</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="3"/>
+        <v>1.208393653324505</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="4"/>
+        <v>0.13639999999999999</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="5"/>
+        <v>2.728E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>100</v>
+      </c>
+      <c r="C7" s="2">
+        <v>838</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="6"/>
+        <v>6.6438561897747253</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="7"/>
+        <v>664.38561897747252</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="9"/>
+        <v>1000000</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="2"/>
+        <v>126.13156818320812</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="3"/>
+        <v>1.2613156818320812</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="4"/>
+        <v>8.3799999999999999E-2</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="5"/>
+        <v>8.3799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>500</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5699</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="6"/>
+        <v>8.965784284662087</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="7"/>
+        <v>4482.8921423310439</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="9"/>
+        <v>125000000</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>11.398</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="2"/>
+        <v>635.63875942781408</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>1.271277518855628</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="4"/>
+        <v>2.2796E-2</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="5"/>
+        <v>4.5592E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12271</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="6"/>
+        <v>9.965784284662087</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="7"/>
+        <v>9965.7842846620879</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="8"/>
+        <v>1000000</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="9"/>
+        <v>1000000000</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>12.271000000000001</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="2"/>
+        <v>1231.3130255975711</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>1.2313130255975711</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="4"/>
+        <v>1.2271000000000001E-2</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="5"/>
+        <v>1.2271E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>5000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>77227</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="6"/>
+        <v>12.287712379549451</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="7"/>
+        <v>61438.561897747255</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="8"/>
+        <v>25000000</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="9"/>
+        <v>125000000000</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>15.445399999999999</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="2"/>
+        <v>6284.8964570923381</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>1.2569792914184674</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="4"/>
+        <v>3.0890800000000001E-3</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="5"/>
+        <v>6.1781599999999995E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C11" s="6">
+        <v>165522</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="6"/>
+        <v>13.287712379549451</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="7"/>
+        <v>132877.1237954945</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="8"/>
+        <v>100000000</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="9"/>
+        <v>1000000000000</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>16.552199999999999</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="2"/>
+        <v>12456.771735573373</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>1.2456771735573373</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="4"/>
+        <v>1.65522E-3</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="5"/>
+        <v>1.6552199999999999E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6EDF7F-5FB0-4BFD-8637-C8A341252F56}">
   <dimension ref="B2:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="123" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -625,7 +1101,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2">
-        <f>B4</f>
+        <f t="shared" ref="D4:D11" si="0">B4</f>
         <v>1</v>
       </c>
       <c r="E4" s="2">
@@ -645,23 +1121,23 @@
         <v>1</v>
       </c>
       <c r="I4" s="2">
-        <f>C4/D4</f>
+        <f t="shared" ref="I4:I11" si="1">C4/D4</f>
         <v>2</v>
       </c>
       <c r="J4" s="2" t="e">
-        <f>C4/E4</f>
+        <f t="shared" ref="J4:J11" si="2">C4/E4</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K4" s="2" t="e">
-        <f>C4/F4</f>
+        <f t="shared" ref="K4:K11" si="3">C4/F4</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L4" s="2">
-        <f>C4/G4</f>
+        <f t="shared" ref="L4:L11" si="4">C4/G4</f>
         <v>2</v>
       </c>
       <c r="M4" s="2">
-        <f>C4/H4</f>
+        <f t="shared" ref="M4:M11" si="5">C4/H4</f>
         <v>2</v>
       </c>
     </row>
@@ -673,43 +1149,43 @@
         <v>8</v>
       </c>
       <c r="D5" s="2">
-        <f>B5</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E11" si="0">LOG(D5,2)</f>
+        <f t="shared" ref="E5:E11" si="6">LOG(D5,2)</f>
         <v>3.3219280948873626</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F11" si="1">D5*E5</f>
+        <f t="shared" ref="F5:F11" si="7">D5*E5</f>
         <v>33.219280948873624</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ref="G5:G11" si="2">POWER(D5,2)</f>
+        <f t="shared" ref="G5:G11" si="8">POWER(D5,2)</f>
         <v>100</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ref="H5:H11" si="3">POWER(D5, 3)</f>
+        <f t="shared" ref="H5:H11" si="9">POWER(D5, 3)</f>
         <v>1000</v>
       </c>
       <c r="I5" s="2">
-        <f>C5/D5</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="J5" s="2">
-        <f>C5/E5</f>
+        <f t="shared" si="2"/>
         <v>2.4082399653118491</v>
       </c>
       <c r="K5" s="2">
-        <f>C5/F5</f>
+        <f t="shared" si="3"/>
         <v>0.24082399653118494</v>
       </c>
       <c r="L5" s="2">
-        <f>C5/G5</f>
+        <f t="shared" si="4"/>
         <v>0.08</v>
       </c>
       <c r="M5" s="2">
-        <f>C5/H5</f>
+        <f t="shared" si="5"/>
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
@@ -721,43 +1197,43 @@
         <v>11</v>
       </c>
       <c r="D6" s="2">
-        <f>B6</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>5.6438561897747244</v>
       </c>
       <c r="F6" s="2">
+        <f t="shared" si="7"/>
+        <v>282.1928094887362</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="8"/>
+        <v>2500</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="9"/>
+        <v>125000</v>
+      </c>
+      <c r="I6" s="2">
         <f t="shared" si="1"/>
-        <v>282.1928094887362</v>
-      </c>
-      <c r="G6" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="J6" s="2">
         <f t="shared" si="2"/>
-        <v>2500</v>
-      </c>
-      <c r="H6" s="2">
+        <v>1.9490220214911371</v>
+      </c>
+      <c r="K6" s="2">
         <f t="shared" si="3"/>
-        <v>125000</v>
-      </c>
-      <c r="I6" s="2">
-        <f>C6/D6</f>
-        <v>0.22</v>
-      </c>
-      <c r="J6" s="2">
-        <f>C6/E6</f>
-        <v>1.9490220214911371</v>
-      </c>
-      <c r="K6" s="2">
-        <f>C6/F6</f>
         <v>3.8980440429822745E-2</v>
       </c>
       <c r="L6" s="2">
-        <f>C6/G6</f>
+        <f t="shared" si="4"/>
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="M6" s="2">
-        <f>C6/H6</f>
+        <f t="shared" si="5"/>
         <v>8.7999999999999998E-5</v>
       </c>
     </row>
@@ -769,43 +1245,43 @@
         <v>17</v>
       </c>
       <c r="D7" s="2">
-        <f>B7</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>6.6438561897747253</v>
       </c>
       <c r="F7" s="2">
+        <f t="shared" si="7"/>
+        <v>664.38561897747252</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="9"/>
+        <v>1000000</v>
+      </c>
+      <c r="I7" s="2">
         <f t="shared" si="1"/>
-        <v>664.38561897747252</v>
-      </c>
-      <c r="G7" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="J7" s="2">
         <f t="shared" si="2"/>
-        <v>10000</v>
-      </c>
-      <c r="H7" s="2">
+        <v>2.5587549631438398</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="3"/>
-        <v>1000000</v>
-      </c>
-      <c r="I7" s="2">
-        <f>C7/D7</f>
-        <v>0.17</v>
-      </c>
-      <c r="J7" s="2">
-        <f>C7/E7</f>
-        <v>2.5587549631438398</v>
-      </c>
-      <c r="K7" s="2">
-        <f>C7/F7</f>
         <v>2.5587549631438399E-2</v>
       </c>
       <c r="L7" s="2">
-        <f>C7/G7</f>
+        <f t="shared" si="4"/>
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="M7" s="2">
-        <f>C7/H7</f>
+        <f t="shared" si="5"/>
         <v>1.7E-5</v>
       </c>
     </row>
@@ -817,43 +1293,43 @@
         <v>20</v>
       </c>
       <c r="D8" s="2">
-        <f>B8</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>8.965784284662087</v>
       </c>
       <c r="F8" s="2">
+        <f t="shared" si="7"/>
+        <v>4482.8921423310439</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="8"/>
+        <v>250000</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="9"/>
+        <v>125000000</v>
+      </c>
+      <c r="I8" s="2">
         <f t="shared" si="1"/>
-        <v>4482.8921423310439</v>
-      </c>
-      <c r="G8" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="J8" s="2">
         <f t="shared" si="2"/>
-        <v>250000</v>
-      </c>
-      <c r="H8" s="2">
+        <v>2.2307027879551291</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="3"/>
-        <v>125000000</v>
-      </c>
-      <c r="I8" s="2">
-        <f>C8/D8</f>
-        <v>0.04</v>
-      </c>
-      <c r="J8" s="2">
-        <f>C8/E8</f>
-        <v>2.2307027879551291</v>
-      </c>
-      <c r="K8" s="2">
-        <f>C8/F8</f>
         <v>4.4614055759102577E-3</v>
       </c>
       <c r="L8" s="2">
-        <f>C8/G8</f>
+        <f t="shared" si="4"/>
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="M8" s="2">
-        <f>C8/H8</f>
+        <f t="shared" si="5"/>
         <v>1.6E-7</v>
       </c>
     </row>
@@ -865,43 +1341,43 @@
         <v>29</v>
       </c>
       <c r="D9" s="2">
-        <f>B9</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>9.965784284662087</v>
       </c>
       <c r="F9" s="2">
+        <f t="shared" si="7"/>
+        <v>9965.7842846620879</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="8"/>
+        <v>1000000</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="9"/>
+        <v>1000000000</v>
+      </c>
+      <c r="I9" s="2">
         <f t="shared" si="1"/>
-        <v>9965.7842846620879</v>
-      </c>
-      <c r="G9" s="2">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="J9" s="2">
         <f t="shared" si="2"/>
-        <v>1000000</v>
-      </c>
-      <c r="H9" s="2">
+        <v>2.909956624751818</v>
+      </c>
+      <c r="K9" s="2">
         <f t="shared" si="3"/>
-        <v>1000000000</v>
-      </c>
-      <c r="I9" s="2">
-        <f>C9/D9</f>
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="J9" s="2">
-        <f>C9/E9</f>
-        <v>2.909956624751818</v>
-      </c>
-      <c r="K9" s="2">
-        <f>C9/F9</f>
         <v>2.909956624751818E-3</v>
       </c>
       <c r="L9" s="2">
-        <f>C9/G9</f>
+        <f t="shared" si="4"/>
         <v>2.9E-5</v>
       </c>
       <c r="M9" s="2">
-        <f>C9/H9</f>
+        <f t="shared" si="5"/>
         <v>2.9000000000000002E-8</v>
       </c>
     </row>
@@ -913,43 +1389,43 @@
         <v>29</v>
       </c>
       <c r="D10" s="2">
-        <f>B10</f>
+        <f t="shared" si="0"/>
         <v>5000</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>12.287712379549451</v>
       </c>
       <c r="F10" s="2">
+        <f t="shared" si="7"/>
+        <v>61438.561897747255</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="8"/>
+        <v>25000000</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="9"/>
+        <v>125000000000</v>
+      </c>
+      <c r="I10" s="2">
         <f t="shared" si="1"/>
-        <v>61438.561897747255</v>
-      </c>
-      <c r="G10" s="2">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="J10" s="2">
         <f t="shared" si="2"/>
-        <v>25000000</v>
-      </c>
-      <c r="H10" s="2">
+        <v>2.360081283173991</v>
+      </c>
+      <c r="K10" s="2">
         <f t="shared" si="3"/>
-        <v>125000000000</v>
-      </c>
-      <c r="I10" s="2">
-        <f>C10/D10</f>
-        <v>5.7999999999999996E-3</v>
-      </c>
-      <c r="J10" s="2">
-        <f>C10/E10</f>
-        <v>2.360081283173991</v>
-      </c>
-      <c r="K10" s="2">
-        <f>C10/F10</f>
         <v>4.7201625663479817E-4</v>
       </c>
       <c r="L10" s="2">
-        <f>C10/G10</f>
+        <f t="shared" si="4"/>
         <v>1.1599999999999999E-6</v>
       </c>
       <c r="M10" s="2">
-        <f>C10/H10</f>
+        <f t="shared" si="5"/>
         <v>2.32E-10</v>
       </c>
     </row>
@@ -961,43 +1437,43 @@
         <v>35</v>
       </c>
       <c r="D11" s="2">
-        <f>B11</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>13.287712379549451</v>
       </c>
       <c r="F11" s="2">
+        <f t="shared" si="7"/>
+        <v>132877.1237954945</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="8"/>
+        <v>100000000</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="9"/>
+        <v>1000000000000</v>
+      </c>
+      <c r="I11" s="2">
         <f t="shared" si="1"/>
-        <v>132877.1237954945</v>
-      </c>
-      <c r="G11" s="2">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="J11" s="2">
         <f t="shared" si="2"/>
-        <v>100000000</v>
-      </c>
-      <c r="H11" s="2">
+        <v>2.6340124620598351</v>
+      </c>
+      <c r="K11" s="2">
         <f t="shared" si="3"/>
-        <v>1000000000000</v>
-      </c>
-      <c r="I11" s="2">
-        <f>C11/D11</f>
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="J11" s="2">
-        <f>C11/E11</f>
-        <v>2.6340124620598351</v>
-      </c>
-      <c r="K11" s="2">
-        <f>C11/F11</f>
         <v>2.6340124620598352E-4</v>
       </c>
       <c r="L11" s="2">
-        <f>C11/G11</f>
+        <f t="shared" si="4"/>
         <v>3.4999999999999998E-7</v>
       </c>
       <c r="M11" s="2">
-        <f>C11/H11</f>
+        <f t="shared" si="5"/>
         <v>3.5000000000000002E-11</v>
       </c>
     </row>
@@ -1010,7 +1486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N21"/>
   <sheetViews>

</xml_diff>

<commit_message>
changed functionality of quicksort and added updated ratio analysis for quicksort
</commit_message>
<xml_diff>
--- a/Ex6/Ex6-RatioAnalysis.xlsx
+++ b/Ex6/Ex6-RatioAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PyCharmProjects\DSALab\Ex6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1E1103-B0A8-4A97-B88C-0A092326758D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5F09FB-4E75-4C24-A3E2-F7232459F448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,10 +228,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,7 +549,7 @@
   <dimension ref="B2:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,20 +569,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="2:13" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -627,7 +627,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ref="D4:D11" si="0">B4</f>
@@ -651,7 +651,7 @@
       </c>
       <c r="I4" s="2">
         <f t="shared" ref="I4:I11" si="1">C4/D4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="2" t="e">
         <f t="shared" ref="J4:J11" si="2">C4/E4</f>
@@ -663,11 +663,11 @@
       </c>
       <c r="L4" s="2">
         <f t="shared" ref="L4:L11" si="4">C4/G4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" ref="M4:M11" si="5">C4/H4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
@@ -675,7 +675,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="2">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
@@ -699,23 +699,23 @@
       </c>
       <c r="I5" s="2">
         <f t="shared" si="1"/>
-        <v>5.6</v>
+        <v>1.6</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="2"/>
-        <v>16.857679757182947</v>
+        <v>4.8164799306236983</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" si="3"/>
-        <v>1.6857679757182946</v>
+        <v>0.48164799306236988</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" si="4"/>
-        <v>0.56000000000000005</v>
+        <v>0.16</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="5"/>
-        <v>5.6000000000000001E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
@@ -723,7 +723,7 @@
         <v>50</v>
       </c>
       <c r="C6" s="2">
-        <v>341</v>
+        <v>194</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
@@ -747,23 +747,23 @@
       </c>
       <c r="I6" s="2">
         <f t="shared" si="1"/>
-        <v>6.82</v>
+        <v>3.88</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="2"/>
-        <v>60.419682666225249</v>
+        <v>34.373661106298236</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" si="3"/>
-        <v>1.208393653324505</v>
+        <v>0.68747322212596473</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" si="4"/>
-        <v>0.13639999999999999</v>
+        <v>7.7600000000000002E-2</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" si="5"/>
-        <v>2.728E-3</v>
+        <v>1.552E-3</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
@@ -771,7 +771,7 @@
         <v>100</v>
       </c>
       <c r="C7" s="2">
-        <v>838</v>
+        <v>593</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
@@ -795,23 +795,23 @@
       </c>
       <c r="I7" s="2">
         <f t="shared" si="1"/>
-        <v>8.3800000000000008</v>
+        <v>5.93</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="2"/>
-        <v>126.13156818320812</v>
+        <v>89.255393714370413</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" si="3"/>
-        <v>1.2613156818320812</v>
+        <v>0.89255393714370412</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" si="4"/>
-        <v>8.3799999999999999E-2</v>
+        <v>5.9299999999999999E-2</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" si="5"/>
-        <v>8.3799999999999999E-4</v>
+        <v>5.9299999999999999E-4</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
@@ -819,7 +819,7 @@
         <v>500</v>
       </c>
       <c r="C8" s="2">
-        <v>5699</v>
+        <v>3914</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
@@ -843,23 +843,23 @@
       </c>
       <c r="I8" s="2">
         <f t="shared" si="1"/>
-        <v>11.398</v>
+        <v>7.8280000000000003</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="2"/>
-        <v>635.63875942781408</v>
+        <v>436.54853560281873</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="3"/>
-        <v>1.271277518855628</v>
+        <v>0.8730970712056374</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="4"/>
-        <v>2.2796E-2</v>
+        <v>1.5656E-2</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="5"/>
-        <v>4.5592E-5</v>
+        <v>3.1312000000000001E-5</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
@@ -867,7 +867,7 @@
         <v>1000</v>
       </c>
       <c r="C9" s="2">
-        <v>12271</v>
+        <v>9225</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
@@ -891,23 +891,23 @@
       </c>
       <c r="I9" s="2">
         <f t="shared" si="1"/>
-        <v>12.271000000000001</v>
+        <v>9.2249999999999996</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="2"/>
-        <v>1231.3130255975711</v>
+        <v>925.66723666674216</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="3"/>
-        <v>1.2313130255975711</v>
+        <v>0.92566723666674211</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" si="4"/>
-        <v>1.2271000000000001E-2</v>
+        <v>9.2250000000000006E-3</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" si="5"/>
-        <v>1.2271E-5</v>
+        <v>9.2250000000000006E-6</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
@@ -915,7 +915,7 @@
         <v>5000</v>
       </c>
       <c r="C10" s="2">
-        <v>77227</v>
+        <v>60487</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
@@ -939,31 +939,31 @@
       </c>
       <c r="I10" s="2">
         <f t="shared" si="1"/>
-        <v>15.445399999999999</v>
+        <v>12.0974</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="2"/>
-        <v>6284.8964570923381</v>
+        <v>4922.5598819084544</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="3"/>
-        <v>1.2569792914184674</v>
+        <v>0.98451197638169086</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" si="4"/>
-        <v>3.0890800000000001E-3</v>
+        <v>2.4194799999999999E-3</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" si="5"/>
-        <v>6.1781599999999995E-7</v>
+        <v>4.8389600000000003E-7</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>10000</v>
       </c>
-      <c r="C11" s="6">
-        <v>165522</v>
+      <c r="C11" s="5">
+        <v>146965</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
@@ -987,23 +987,23 @@
       </c>
       <c r="I11" s="2">
         <f t="shared" si="1"/>
-        <v>16.552199999999999</v>
+        <v>14.6965</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="2"/>
-        <v>12456.771735573373</v>
+        <v>11060.218328189248</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="3"/>
-        <v>1.2456771735573373</v>
+        <v>1.1060218328189249</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" si="4"/>
-        <v>1.65522E-3</v>
+        <v>1.4696500000000001E-3</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" si="5"/>
-        <v>1.6552199999999999E-7</v>
+        <v>1.4696499999999999E-7</v>
       </c>
     </row>
   </sheetData>
@@ -1040,20 +1040,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="2:13" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -1511,21 +1511,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="2:14" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">

</xml_diff>